<commit_message>
Added gaseous swelling model to VSwellingUC
</commit_message>
<xml_diff>
--- a/tests/materials/VSwellingUC/solidswellingUC.xlsx
+++ b/tests/materials/VSwellingUC/solidswellingUC.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-11160" yWindow="-18160" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="solid" sheetId="1" r:id="rId1"/>
+    <sheet name="gas" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="29">
   <si>
     <t>DV/v</t>
   </si>
@@ -45,16 +46,78 @@
     <t>swelling_factor*Fsn/atom</t>
   </si>
   <si>
-    <t>|</t>
+    <t>time</t>
+  </si>
+  <si>
+    <t>burnup</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>zone</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>F01</t>
+  </si>
+  <si>
+    <t>a/o</t>
+  </si>
+  <si>
+    <t>% per a/o</t>
+  </si>
+  <si>
+    <t>mu2+</t>
+  </si>
+  <si>
+    <t>S2+</t>
+  </si>
+  <si>
+    <t>F02</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>K2*</t>
+  </si>
+  <si>
+    <t>P2 zone 3</t>
+  </si>
+  <si>
+    <t>P2 zone 4</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>diff [%]</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000000000"/>
-    <numFmt numFmtId="167" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="169" formatCode="0.0000E+00"/>
+    <numFmt numFmtId="171" formatCode="0.000000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -62,6 +125,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -105,7 +169,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="74">
+  <cellStyleXfs count="162">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -180,15 +244,107 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="74">
+  <cellStyles count="162">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -225,6 +381,50 @@
     <cellStyle name="Followed Hyperlink" xfId="69" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="71" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="73" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="75" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="77" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="79" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="81" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="83" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="85" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="87" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="89" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="91" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="93" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="95" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="97" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="99" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="101" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="103" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="105" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="107" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="109" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="111" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="113" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="115" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="117" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="119" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="121" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="123" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="125" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="127" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="129" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="131" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="133" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="135" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="137" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="139" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="141" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="143" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="145" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="147" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="149" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="151" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="153" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="155" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="157" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="159" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="161" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -261,6 +461,50 @@
     <cellStyle name="Hyperlink" xfId="68" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="70" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="72" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="74" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="76" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="78" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="80" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="82" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="84" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="86" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="88" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="90" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="92" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="94" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="96" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="98" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="100" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="102" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="104" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="106" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="108" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="110" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="112" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="114" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="116" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="118" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="120" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="122" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="124" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="126" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="128" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="130" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="132" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="134" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="136" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="138" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="140" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="142" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="144" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="146" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="148" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="150" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="152" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="154" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="156" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="158" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="160" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -591,10 +835,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N32"/>
+  <dimension ref="A2:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -720,387 +964,577 @@
         <v>2.5427007651333947E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:5">
       <c r="A17" s="3"/>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:5">
       <c r="A18" s="3"/>
     </row>
-    <row r="19" spans="1:14">
-      <c r="C19" t="s">
+    <row r="19" spans="1:5">
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="C22" s="3"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="D32" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D2:N30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28:L28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="8" max="8" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:14">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="4:14">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <v>1.5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="4:14">
+      <c r="D5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E5">
+        <v>0.61299999999999999</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="4:14">
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>0.83</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="4:14">
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7">
+        <v>1.8E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="4:14">
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="4:14">
+      <c r="F10" t="s">
+        <v>12</v>
+      </c>
+      <c r="G10">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="12" spans="4:14">
+      <c r="D12" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="3">
-        <v>37000000</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="E12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+      <c r="I12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K12" t="s">
+        <v>24</v>
+      </c>
+      <c r="L12" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" t="s">
+        <v>26</v>
+      </c>
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="4:14">
+      <c r="D13" s="3">
+        <v>10000000</v>
+      </c>
+      <c r="E13" s="3">
+        <v>1221.01</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3.6543699999999998E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>4</v>
+      </c>
+      <c r="H13" s="7">
+        <v>1.0169410000000001</v>
+      </c>
+      <c r="I13" s="8">
+        <f>$E$2*($F13*100-$E$3)</f>
+        <v>6.8939839999999988E-2</v>
+      </c>
+      <c r="J13" s="5">
+        <f>$E$5*($F13*100-$E$6)</f>
+        <v>1.7313388099999998</v>
+      </c>
+      <c r="K13" s="4">
+        <f>$J13-$E$7*($F13*100-$E$6)*($E13-$G$10)</f>
+        <v>1.6245267853399998</v>
+      </c>
+      <c r="L13" s="5">
+        <f>$J13-$E$8*($F13*100-$E$6)*($E13-$G$10)</f>
+        <v>0.90057861820000029</v>
+      </c>
+      <c r="M13" s="8">
+        <f>(I13+K13)/100+1</f>
+        <v>1.0169346662534</v>
+      </c>
+      <c r="N13" s="7">
+        <f>ABS(H13-M13)/M13*100</f>
+        <v>6.2282728775678515E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="4:14">
+      <c r="D14" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="E14" s="3">
+        <v>1164.404</v>
+      </c>
+      <c r="F14" s="3">
+        <v>7.3087399999999997E-2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1.073925</v>
+      </c>
+      <c r="I14" s="8">
+        <f>$E$2*($F14*100-$E$3)</f>
+        <v>0.18587967999999999</v>
+      </c>
+      <c r="J14" s="5">
+        <f>$E$5*($F14*100-$E$6)</f>
+        <v>3.9714676199999994</v>
+      </c>
+      <c r="K14" s="4">
+        <f t="shared" ref="K14:K18" si="0">$J14-$E$7*($F14*100-$E$6)*($E14-$G$10)</f>
+        <v>4.3865786322719993</v>
+      </c>
+      <c r="L14" s="5">
+        <f t="shared" ref="L14:L18" si="1">$J14-$E$8*($F14*100-$E$6)*($E14-$G$10)</f>
+        <v>7.2001088265599993</v>
+      </c>
+      <c r="M14" s="8">
+        <f>(I14+L14)/100+1</f>
+        <v>1.0738598850656</v>
+      </c>
+      <c r="N14" s="7">
+        <f t="shared" ref="N14:N16" si="2">ABS(H14-M14)/M14*100</f>
+        <v>6.0636341207588092E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="4:14">
+      <c r="D15" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="E15" s="3">
+        <v>1133.6610000000001</v>
+      </c>
+      <c r="F15" s="3">
+        <v>0.1096311</v>
+      </c>
+      <c r="G15" s="3">
+        <v>3</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1.1594370000000001</v>
+      </c>
+      <c r="I15" s="8">
+        <f>$E$2*($F15*100-$E$3)</f>
+        <v>0.30281952000000001</v>
+      </c>
+      <c r="J15" s="5">
+        <f>$E$5*($F15*100-$E$6)</f>
+        <v>6.2115964300000002</v>
+      </c>
+      <c r="K15" s="4">
+        <f t="shared" si="0"/>
+        <v>7.4215931217219993</v>
+      </c>
+      <c r="L15" s="5">
+        <f t="shared" si="1"/>
+        <v>15.622681810059992</v>
+      </c>
+      <c r="M15" s="8">
+        <f>(I15+L15)/100+1</f>
+        <v>1.1592550133005999</v>
+      </c>
+      <c r="N15" s="7">
+        <f t="shared" si="2"/>
+        <v>1.5698590673507123E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="4:14">
+      <c r="D16" s="3">
+        <v>40000000</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1112.8140000000001</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.14617479999999999</v>
+      </c>
+      <c r="G16" s="3">
+        <v>3</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1.257333</v>
+      </c>
+      <c r="I16" s="8">
+        <f>$E$2*($F16*100-$E$3)</f>
+        <v>0.41975935999999997</v>
+      </c>
+      <c r="J16" s="5">
+        <f>$E$5*($F16*100-$E$6)</f>
+        <v>8.4517252399999983</v>
+      </c>
+      <c r="K16" s="4">
+        <f t="shared" si="0"/>
+        <v>10.615460656303997</v>
+      </c>
+      <c r="L16" s="5">
+        <f t="shared" si="1"/>
+        <v>25.280778477919981</v>
+      </c>
+      <c r="M16" s="8">
+        <f>(I16+L16)/100+1</f>
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="N16" s="7">
+        <f t="shared" si="2"/>
+        <v>2.6063661018107458E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14">
+      <c r="D17" s="3">
+        <v>50000000</v>
+      </c>
+      <c r="E17" s="3">
+        <v>1097.165</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.18271850000000001</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1.3311539999999999</v>
+      </c>
+      <c r="I17" s="8">
+        <f>$E$2*($F17*100-$E$3)</f>
+        <v>0.53669920000000004</v>
+      </c>
+      <c r="J17" s="5">
+        <f>$E$5*($F17*100-$E$6)</f>
+        <v>10.691854050000002</v>
+      </c>
+      <c r="K17" s="4">
+        <f t="shared" si="0"/>
+        <v>13.920392810550004</v>
+      </c>
+      <c r="L17" s="5">
+        <f t="shared" si="1"/>
+        <v>35.802711076500017</v>
+      </c>
+      <c r="M17" s="8">
+        <f>M16</f>
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="N17" s="7"/>
+    </row>
+    <row r="18" spans="4:14">
+      <c r="D18" s="3">
+        <v>60000000</v>
+      </c>
+      <c r="E18" s="3">
+        <v>1084.702</v>
+      </c>
+      <c r="F18" s="3">
+        <v>0.21926219999999999</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="7">
+        <v>1.3311539999999999</v>
+      </c>
+      <c r="I18" s="8">
+        <f>$E$2*($F18*100-$E$3)</f>
+        <v>0.65363904000000006</v>
+      </c>
+      <c r="J18" s="5">
+        <f>$E$5*($F18*100-$E$6)</f>
+        <v>12.931982860000002</v>
+      </c>
+      <c r="K18" s="4">
+        <f t="shared" si="0"/>
+        <v>17.310216412408003</v>
+      </c>
+      <c r="L18" s="5">
+        <f t="shared" si="1"/>
+        <v>46.984910489840004</v>
+      </c>
+      <c r="M18" s="8">
+        <f>M17</f>
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="N18" s="7"/>
+    </row>
+    <row r="19" spans="4:14">
+      <c r="G19" s="6"/>
+      <c r="M19" s="8"/>
+    </row>
+    <row r="21" spans="4:14">
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="4:14">
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F19" s="3">
-        <v>0.13521169999999999</v>
-      </c>
-      <c r="G19" t="s">
-        <v>8</v>
-      </c>
-      <c r="H19" s="3">
-        <v>1.067626</v>
-      </c>
-      <c r="I19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="C20" t="s">
-        <v>8</v>
-      </c>
-      <c r="D20" s="3">
-        <v>38000000</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-      <c r="F20" s="3">
-        <v>0.13886609999999999</v>
-      </c>
-      <c r="G20" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="3">
-        <v>1.0694539999999999</v>
-      </c>
-      <c r="I20" t="s">
-        <v>8</v>
-      </c>
-      <c r="L20" s="3">
-        <v>0</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="D21" s="3">
-        <v>39000000</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-      <c r="F21" s="3">
-        <v>0.14252039999999999</v>
-      </c>
-      <c r="G21" t="s">
-        <v>8</v>
-      </c>
-      <c r="H21" s="3">
-        <v>1.0712820000000001</v>
-      </c>
-      <c r="I21" t="s">
-        <v>8</v>
-      </c>
-      <c r="L21" s="3">
+      <c r="J22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14">
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H23" s="3">
         <v>10000000</v>
       </c>
-      <c r="M21" s="3">
-        <v>3.6543699999999998E-2</v>
-      </c>
-      <c r="N21" s="3">
-        <v>1.0182770000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14">
-      <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D22" s="1">
+      <c r="I23" s="7">
+        <v>1.0169410000000001</v>
+      </c>
+      <c r="J23">
+        <v>1.0169346662534</v>
+      </c>
+      <c r="K23">
+        <v>6.2282728775678515E-4</v>
+      </c>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="4:14">
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="3">
+        <v>20000000</v>
+      </c>
+      <c r="I24" s="7">
+        <v>1.073925</v>
+      </c>
+      <c r="J24">
+        <v>1.0738598850656</v>
+      </c>
+      <c r="K24">
+        <v>6.0636341207588092E-3</v>
+      </c>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="4:14">
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="I25" s="7">
+        <v>1.1594370000000001</v>
+      </c>
+      <c r="J25">
+        <v>1.1592550133005999</v>
+      </c>
+      <c r="K25">
+        <v>1.5698590673507123E-2</v>
+      </c>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="4:14">
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="3">
         <v>40000000</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="3">
-        <v>0.14617479999999999</v>
-      </c>
-      <c r="G22" t="s">
-        <v>8</v>
-      </c>
-      <c r="H22" s="3">
-        <v>1.0731090000000001</v>
-      </c>
-      <c r="I22" t="s">
-        <v>8</v>
-      </c>
-      <c r="L22" s="3">
-        <v>20000000</v>
-      </c>
-      <c r="M22" s="3">
-        <v>7.3087399999999997E-2</v>
-      </c>
-      <c r="N22" s="3">
-        <v>1.0365549999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14">
-      <c r="C23" t="s">
-        <v>8</v>
-      </c>
-      <c r="D23" s="3">
-        <v>41000000</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="3">
-        <v>0.1498292</v>
-      </c>
-      <c r="G23" t="s">
-        <v>8</v>
-      </c>
-      <c r="H23" s="3">
-        <v>1.074937</v>
-      </c>
-      <c r="I23" t="s">
-        <v>8</v>
-      </c>
-      <c r="L23" s="3">
-        <v>30000000</v>
-      </c>
-      <c r="M23" s="3">
-        <v>0.1096311</v>
-      </c>
-      <c r="N23" s="3">
-        <v>1.054832</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14">
-      <c r="C24" t="s">
-        <v>8</v>
-      </c>
-      <c r="D24" s="3">
-        <v>42000000</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0.15348349999999999</v>
-      </c>
-      <c r="G24" t="s">
-        <v>8</v>
-      </c>
-      <c r="H24" s="3">
-        <v>1.076765</v>
-      </c>
-      <c r="I24" t="s">
-        <v>8</v>
-      </c>
-      <c r="L24" s="3">
-        <v>40000000</v>
-      </c>
-      <c r="M24" s="3">
-        <v>0.14617479999999999</v>
-      </c>
-      <c r="N24" s="3">
-        <v>1.0731090000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14">
-      <c r="C25" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="3">
-        <v>43000000</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0.1571379</v>
-      </c>
-      <c r="G25" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="3">
-        <v>1.0785929999999999</v>
-      </c>
-      <c r="I25" t="s">
-        <v>8</v>
-      </c>
-      <c r="L25" s="3">
+      <c r="I26" s="7">
+        <v>1.257333</v>
+      </c>
+      <c r="J26">
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="K26">
+        <v>2.6063661018107458E-2</v>
+      </c>
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="4:14">
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="3">
         <v>50000000</v>
       </c>
-      <c r="M25" s="3">
-        <v>0.18271850000000001</v>
-      </c>
-      <c r="N25" s="3">
-        <v>1.0913870000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14">
-      <c r="C26" t="s">
-        <v>8</v>
-      </c>
-      <c r="D26" s="3">
-        <v>44000000</v>
-      </c>
-      <c r="E26" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="3">
-        <v>0.1607923</v>
-      </c>
-      <c r="G26" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="3">
-        <v>1.0804199999999999</v>
-      </c>
-      <c r="I26" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14">
-      <c r="C27" t="s">
-        <v>8</v>
-      </c>
-      <c r="D27" s="3">
-        <v>45000000</v>
-      </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0.1644467</v>
-      </c>
-      <c r="G27" t="s">
-        <v>8</v>
-      </c>
-      <c r="H27" s="3">
-        <v>1.0822480000000001</v>
-      </c>
-      <c r="I27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14">
-      <c r="C28" t="s">
-        <v>8</v>
-      </c>
-      <c r="D28" s="3">
-        <v>46000000</v>
-      </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0.168101</v>
-      </c>
-      <c r="G28" t="s">
-        <v>8</v>
+      <c r="I27" s="7">
+        <v>1.3311539999999999</v>
+      </c>
+      <c r="J27">
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="4:14">
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="H28" s="3">
-        <v>1.084076</v>
-      </c>
-      <c r="I28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14">
-      <c r="C29" t="s">
-        <v>8</v>
-      </c>
-      <c r="D29" s="3">
-        <v>47000000</v>
-      </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0.1717554</v>
-      </c>
-      <c r="G29" t="s">
-        <v>8</v>
-      </c>
-      <c r="H29" s="3">
-        <v>1.085904</v>
-      </c>
-      <c r="I29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14">
-      <c r="C30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3">
-        <v>48000000</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0.1754098</v>
-      </c>
-      <c r="G30" t="s">
-        <v>8</v>
-      </c>
-      <c r="H30" s="3">
-        <v>1.087731</v>
-      </c>
-      <c r="I30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14">
-      <c r="C31" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="3">
-        <v>49000000</v>
-      </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-      <c r="F31" s="3">
-        <v>0.1790641</v>
-      </c>
-      <c r="G31" t="s">
-        <v>8</v>
-      </c>
-      <c r="H31" s="3">
-        <v>1.0895589999999999</v>
-      </c>
-      <c r="I31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14">
-      <c r="C32" t="s">
-        <v>8</v>
-      </c>
-      <c r="D32" s="3">
-        <v>50000000</v>
-      </c>
-      <c r="E32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0.18271850000000001</v>
-      </c>
-      <c r="G32" t="s">
-        <v>8</v>
-      </c>
-      <c r="H32" s="3">
-        <v>1.0913870000000001</v>
-      </c>
-      <c r="I32" t="s">
-        <v>8</v>
-      </c>
+        <v>60000000</v>
+      </c>
+      <c r="I28" s="7">
+        <v>1.3311539999999999</v>
+      </c>
+      <c r="J28">
+        <v>1.2570053783791999</v>
+      </c>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="4:14">
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="4:14">
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>